<commit_message>
This is the updated code of EOA DDF Framework!
</commit_message>
<xml_diff>
--- a/src/test/resources/TestExcel.xlsx
+++ b/src/test/resources/TestExcel.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11430" windowHeight="2670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Testcases" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>LoginTest</t>
   </si>
@@ -48,9 +49,6 @@
   </si>
   <si>
     <t>Runmode</t>
-  </si>
-  <si>
-    <t>Firefox</t>
   </si>
   <si>
     <t>Failure</t>
@@ -507,10 +505,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -531,7 +529,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -539,7 +537,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -555,19 +553,19 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -600,10 +598,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>9</v>
@@ -614,16 +612,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="6">
         <v>12345678</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -631,10 +629,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="6">
         <v>1234567</v>
@@ -645,7 +643,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -656,22 +654,22 @@
         <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="H8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>7</v>
@@ -685,10 +683,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" s="2">
         <v>12345</v>
@@ -700,7 +698,7 @@
         <v>7234567890</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>9</v>
@@ -714,10 +712,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2">
         <v>12345</v>
@@ -729,7 +727,7 @@
         <v>8234567891</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>9</v>
@@ -743,10 +741,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2">
         <v>12345</v>
@@ -758,7 +756,7 @@
         <v>9234567892</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>9</v>
@@ -772,10 +770,10 @@
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="2">
         <v>12345</v>
@@ -787,7 +785,7 @@
         <v>6234567893</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>9</v>

</xml_diff>